<commit_message>
Adding test for each major functionality
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 2/Planning.xlsx
+++ b/Documentation/Sprint 2/Planning.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C46B17D-2E29-48B4-A17E-7B5D13D12059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9155D8-B39D-45EF-AF88-E686A8CA5204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="3345" windowWidth="21600" windowHeight="11385" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>low</t>
   </si>
   <si>
-    <t>To be during sprint 2</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>We only have one week for this sprint. It might be difficult to make a good quality page.</t>
+  </si>
+  <si>
+    <t>To be during sprint 3</t>
   </si>
 </sst>
 </file>
@@ -532,158 +532,56 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -715,56 +613,158 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31:H34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,20 +1077,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
     </row>
     <row r="2" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1117,21 +1117,21 @@
       <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="I2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="49"/>
+      <c r="L2" s="63"/>
     </row>
     <row r="3" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -1151,19 +1151,19 @@
       <c r="H3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="91" t="s">
+      <c r="I3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="29" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="30"/>
+      <c r="L3" s="81"/>
     </row>
     <row r="4" spans="1:12" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2">
         <v>4</v>
@@ -1183,17 +1183,17 @@
       <c r="H4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="91" t="s">
+      <c r="I4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="84"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="83"/>
     </row>
     <row r="5" spans="1:12" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="84"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
@@ -1210,20 +1210,20 @@
       <c r="G5" s="2">
         <v>3</v>
       </c>
-      <c r="H5" s="88" t="s">
+      <c r="H5" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="91" t="s">
+      <c r="I5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="84"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="83"/>
     </row>
     <row r="6" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2">
         <v>6</v>
@@ -1240,20 +1240,20 @@
       <c r="G6" s="2">
         <v>3</v>
       </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="91" t="s">
+      <c r="H6" s="32"/>
+      <c r="I6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="32"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="83"/>
     </row>
     <row r="7" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="92" t="s">
-        <v>46</v>
+      <c r="B7" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1270,19 +1270,19 @@
       <c r="G7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="98" t="s">
+      <c r="H7" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="96"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="32"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="83"/>
     </row>
     <row r="8" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="93"/>
-      <c r="B8" s="93"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="3">
         <v>2</v>
       </c>
@@ -1298,17 +1298,17 @@
       <c r="G8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="99"/>
-      <c r="I8" s="95" t="s">
+      <c r="H8" s="34"/>
+      <c r="I8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="96"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="32"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="83"/>
     </row>
     <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="93"/>
-      <c r="B9" s="93"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="3">
         <v>3</v>
       </c>
@@ -1324,34 +1324,34 @@
       <c r="G9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="99"/>
-      <c r="I9" s="97" t="s">
+      <c r="H9" s="34"/>
+      <c r="I9" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="96"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="32"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="83"/>
     </row>
     <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="94"/>
-      <c r="B10" s="94"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="3"/>
       <c r="D10" s="12"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="100"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="32"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="83"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2">
         <v>7</v>
@@ -1365,23 +1365,23 @@
       <c r="F11" s="2">
         <v>5</v>
       </c>
-      <c r="G11" s="85" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="88" t="s">
+      <c r="G11" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="84"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="32"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="83"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2">
         <v>8</v>
@@ -1395,19 +1395,19 @@
       <c r="F12" s="2">
         <v>5</v>
       </c>
-      <c r="G12" s="86"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="84" t="s">
+      <c r="G12" s="37"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="84"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="32"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="83"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="84"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2">
         <v>9</v>
@@ -1421,37 +1421,37 @@
       <c r="F13" s="2">
         <v>2</v>
       </c>
-      <c r="G13" s="86"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="84" t="s">
+      <c r="G13" s="37"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="84"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="32"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="83"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="84"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="11"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="34"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="84"/>
+      <c r="L14" s="85"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7">
         <v>10</v>
@@ -1465,25 +1465,25 @@
       <c r="F15" s="7">
         <v>3</v>
       </c>
-      <c r="G15" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="81" t="s">
+      <c r="G15" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="75" t="s">
+      <c r="I15" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="76"/>
-      <c r="K15" s="50" t="s">
+      <c r="J15" s="42"/>
+      <c r="K15" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="51"/>
+      <c r="L15" s="65"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7">
         <v>11</v>
@@ -1497,22 +1497,22 @@
       <c r="F16" s="7">
         <v>3</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="77" t="s">
+      <c r="G16" s="45"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="74"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="53"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="D17" s="13">
         <v>45207</v>
@@ -1523,17 +1523,17 @@
       <c r="F17" s="7">
         <v>2</v>
       </c>
-      <c r="G17" s="79"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="74" t="s">
+      <c r="G17" s="45"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="74"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="53"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7">
         <v>13</v>
@@ -1541,19 +1541,19 @@
       <c r="D18" s="13"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="55"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="69"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="50" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="5">
         <v>14</v>
@@ -1567,25 +1567,25 @@
       <c r="F19" s="5">
         <v>3</v>
       </c>
-      <c r="G19" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="71" t="s">
+      <c r="G19" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="70" t="s">
+      <c r="I19" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="35" t="s">
+      <c r="J19" s="50"/>
+      <c r="K19" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="L19" s="36"/>
+      <c r="L19" s="87"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5">
         <v>15</v>
@@ -1599,19 +1599,19 @@
       <c r="F20" s="5">
         <v>3</v>
       </c>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="70" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="70"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="89"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="5">
         <v>16</v>
@@ -1625,39 +1625,37 @@
       <c r="F21" s="5">
         <v>2</v>
       </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="70" t="s">
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="70"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="38"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="89"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="70"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="14"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="38"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="89"/>
     </row>
     <row r="23" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="6">
-        <v>7</v>
-      </c>
+      <c r="B23" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="6"/>
       <c r="D23" s="15">
         <v>45234</v>
       </c>
@@ -1667,49 +1665,45 @@
       <c r="F23" s="6">
         <v>2</v>
       </c>
-      <c r="G23" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="66" t="s">
+      <c r="G23" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="66"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="38"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="89"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="6">
-        <v>8</v>
-      </c>
+      <c r="A24" s="55"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="15">
         <v>45236</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F24" s="6">
         <v>1</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="66" t="s">
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="66"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="38"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="89"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="6">
-        <v>9</v>
-      </c>
+      <c r="A25" s="55"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="15">
         <v>45234</v>
       </c>
@@ -1719,39 +1713,39 @@
       <c r="F25" s="6">
         <v>1</v>
       </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="66" t="s">
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="66"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="38"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="89"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="56"/>
       <c r="C26" s="6"/>
       <c r="D26" s="15">
         <v>45236</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="38"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="89"/>
     </row>
     <row r="27" spans="1:12" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="67" t="s">
+      <c r="A27" s="58" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="5">
         <v>17</v>
@@ -1765,23 +1759,23 @@
       <c r="F27" s="5">
         <v>3</v>
       </c>
-      <c r="G27" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="71" t="s">
+      <c r="G27" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="I27" s="70" t="s">
+      <c r="I27" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="70"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="38"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="89"/>
     </row>
     <row r="28" spans="1:12" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="68"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="5">
         <v>18</v>
@@ -1795,19 +1789,19 @@
       <c r="F28" s="5">
         <v>3</v>
       </c>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="70" t="s">
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="70"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="38"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="89"/>
     </row>
     <row r="29" spans="1:12" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="5">
         <v>19</v>
@@ -1821,39 +1815,37 @@
       <c r="F29" s="5">
         <v>2</v>
       </c>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="70" t="s">
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="70"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="38"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="89"/>
     </row>
     <row r="30" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="22"/>
       <c r="C30" s="5"/>
       <c r="D30" s="14"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="38"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="89"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="6">
-        <v>4</v>
-      </c>
+      <c r="B31" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="6"/>
       <c r="D31" s="15">
         <v>45234</v>
       </c>
@@ -1863,25 +1855,23 @@
       <c r="F31" s="6">
         <v>2</v>
       </c>
-      <c r="G31" s="26" t="s">
+      <c r="G31" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="I31" s="66" t="s">
+      <c r="I31" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="J31" s="66"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="38"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="89"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="6">
-        <v>5</v>
-      </c>
+      <c r="A32" s="55"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="15">
         <v>45236</v>
       </c>
@@ -1891,21 +1881,19 @@
       <c r="F32" s="6">
         <v>1</v>
       </c>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="66" t="s">
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="J32" s="66"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="38"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="89"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="6">
-        <v>6</v>
-      </c>
+      <c r="A33" s="55"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="15">
         <v>45234</v>
       </c>
@@ -1915,35 +1903,35 @@
       <c r="F33" s="6">
         <v>1</v>
       </c>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="66" t="s">
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="66"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="38"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="89"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="6"/>
       <c r="D34" s="15"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="66"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="40"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="91"/>
     </row>
     <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="74" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="4">
         <v>20</v>
@@ -1957,25 +1945,25 @@
       <c r="F35" s="4">
         <v>2</v>
       </c>
-      <c r="G35" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" s="60" t="s">
+      <c r="G35" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="57" t="s">
+      <c r="I35" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="57"/>
-      <c r="K35" s="41" t="s">
+      <c r="J35" s="71"/>
+      <c r="K35" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="L35" s="42"/>
+      <c r="L35" s="93"/>
     </row>
     <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="61"/>
+      <c r="A36" s="75"/>
       <c r="B36" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="4">
         <v>21</v>
@@ -1989,19 +1977,19 @@
       <c r="F36" s="4">
         <v>2</v>
       </c>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="57" t="s">
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="J36" s="57"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="44"/>
+      <c r="J36" s="71"/>
+      <c r="K36" s="94"/>
+      <c r="L36" s="95"/>
     </row>
     <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="61"/>
+      <c r="A37" s="75"/>
       <c r="B37" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="4">
         <v>21</v>
@@ -2015,34 +2003,34 @@
       <c r="F37" s="4">
         <v>1</v>
       </c>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="57" t="s">
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="J37" s="57"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="44"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="94"/>
+      <c r="L37" s="95"/>
     </row>
     <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="4"/>
       <c r="C38" s="18"/>
       <c r="D38" s="16"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="44"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="95"/>
     </row>
     <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="58" t="s">
+      <c r="A39" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="63"/>
+      <c r="B39" s="98"/>
       <c r="C39" s="19"/>
       <c r="D39" s="17"/>
       <c r="E39" s="10" t="s">
@@ -2051,16 +2039,16 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
-      <c r="I39" s="59" t="s">
+      <c r="I39" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="J39" s="59"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="44"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="94"/>
+      <c r="L39" s="95"/>
     </row>
     <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="58"/>
-      <c r="B40" s="64"/>
+      <c r="A40" s="72"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="19"/>
       <c r="D40" s="17"/>
       <c r="E40" s="10" t="s">
@@ -2069,16 +2057,16 @@
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
-      <c r="I40" s="59" t="s">
+      <c r="I40" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="59"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="44"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="94"/>
+      <c r="L40" s="95"/>
     </row>
     <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
-      <c r="B41" s="64"/>
+      <c r="A41" s="72"/>
+      <c r="B41" s="99"/>
       <c r="C41" s="19"/>
       <c r="D41" s="17"/>
       <c r="E41" s="10" t="s">
@@ -2087,32 +2075,32 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
-      <c r="I41" s="59" t="s">
+      <c r="I41" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="59"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="44"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="94"/>
+      <c r="L41" s="95"/>
     </row>
     <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="58"/>
-      <c r="B42" s="65"/>
+      <c r="A42" s="72"/>
+      <c r="B42" s="100"/>
       <c r="C42" s="19"/>
       <c r="D42" s="17"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="44"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="94"/>
+      <c r="L42" s="95"/>
     </row>
     <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="23"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="18"/>
       <c r="D43" s="16"/>
       <c r="E43" s="4" t="s">
@@ -2121,16 +2109,16 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="57" t="s">
+      <c r="I43" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="J43" s="57"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="44"/>
+      <c r="J43" s="71"/>
+      <c r="K43" s="94"/>
+      <c r="L43" s="95"/>
     </row>
     <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="70"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="18"/>
       <c r="D44" s="16"/>
       <c r="E44" s="4" t="s">
@@ -2139,16 +2127,16 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="57" t="s">
+      <c r="I44" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="J44" s="57"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="44"/>
+      <c r="J44" s="71"/>
+      <c r="K44" s="94"/>
+      <c r="L44" s="95"/>
     </row>
     <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="70"/>
+      <c r="B45" s="78"/>
       <c r="C45" s="18"/>
       <c r="D45" s="16"/>
       <c r="E45" s="4" t="s">
@@ -2157,26 +2145,26 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="57" t="s">
+      <c r="I45" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="57"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="44"/>
+      <c r="J45" s="71"/>
+      <c r="K45" s="94"/>
+      <c r="L45" s="95"/>
     </row>
     <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
-      <c r="B46" s="25"/>
+      <c r="A46" s="70"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="18"/>
       <c r="D46" s="16"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="46"/>
+      <c r="I46" s="71"/>
+      <c r="J46" s="71"/>
+      <c r="K46" s="96"/>
+      <c r="L46" s="97"/>
     </row>
   </sheetData>
   <autoFilter ref="C2:L46" xr:uid="{784DA642-760B-4062-9544-643C79FF24CC}">
@@ -2184,61 +2172,18 @@
     <filterColumn colId="9" showButton="0"/>
   </autoFilter>
   <mergeCells count="83">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="H27:H30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="K3:L14"/>
+    <mergeCell ref="K19:L34"/>
+    <mergeCell ref="K35:L46"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="B39:B42"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K15:L18"/>
@@ -2255,18 +2200,61 @@
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="I35:J35"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="K3:L14"/>
-    <mergeCell ref="K19:L34"/>
-    <mergeCell ref="K35:L46"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="B7:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>